<commit_message>
Finished fixing queries, everything correct
</commit_message>
<xml_diff>
--- a/MalpicaNew.xlsx
+++ b/MalpicaNew.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alons\IdeaProjects\javaExcelImporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20E92A9-50B3-49A4-AF6C-F2A51EB58C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F318CBBC-1B0D-4ACB-A10F-151A41A341C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Malpica" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2995" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2995" uniqueCount="655">
   <si>
     <t>Número</t>
   </si>
@@ -2001,6 +2001,9 @@
   </si>
   <si>
     <t>Cobre</t>
+  </si>
+  <si>
+    <t>Sierra de Xalostoc, Villa de Ayala</t>
   </si>
 </sst>
 </file>
@@ -2479,8 +2482,8 @@
   </sheetPr>
   <dimension ref="A1:V94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F97" workbookViewId="0">
-      <selection activeCell="N53" sqref="N53"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3855,7 +3858,7 @@
         <v>126</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>127</v>
+        <v>547</v>
       </c>
       <c r="H24" s="14"/>
       <c r="I24" s="14" t="s">
@@ -4276,7 +4279,7 @@
       </c>
       <c r="I31" s="14"/>
       <c r="J31" s="14" t="s">
-        <v>181</v>
+        <v>233</v>
       </c>
       <c r="K31" s="14" t="s">
         <v>593</v>
@@ -5404,7 +5407,7 @@
       <c r="F50" s="14"/>
       <c r="G50" s="14"/>
       <c r="H50" s="14" t="s">
-        <v>317</v>
+        <v>654</v>
       </c>
       <c r="I50" s="14" t="s">
         <v>318</v>
@@ -5763,7 +5766,7 @@
         <v>358</v>
       </c>
       <c r="I56" s="14" t="s">
-        <v>359</v>
+        <v>457</v>
       </c>
       <c r="J56" s="14" t="s">
         <v>22</v>
@@ -5821,7 +5824,7 @@
         <v>363</v>
       </c>
       <c r="I57" s="14" t="s">
-        <v>359</v>
+        <v>457</v>
       </c>
       <c r="J57" s="14" t="s">
         <v>22</v>
@@ -6102,7 +6105,7 @@
       </c>
       <c r="G63" s="14"/>
       <c r="H63" s="14" t="s">
-        <v>386</v>
+        <v>106</v>
       </c>
       <c r="I63" s="14"/>
       <c r="J63" s="14" t="s">
@@ -6552,7 +6555,7 @@
       <c r="H72" s="14"/>
       <c r="I72" s="14"/>
       <c r="J72" s="14" t="s">
-        <v>411</v>
+        <v>369</v>
       </c>
       <c r="K72" s="14" t="s">
         <v>588</v>
@@ -7035,7 +7038,7 @@
       <c r="G82" s="14"/>
       <c r="H82" s="14"/>
       <c r="I82" s="14" t="s">
-        <v>438</v>
+        <v>114</v>
       </c>
       <c r="J82" s="14" t="s">
         <v>22</v>
@@ -7571,6 +7574,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>